<commit_message>
export pengadaan penerimaan barang habis pakai meng export data yang sudah di beli (ada di permohonan/pengadaan habis pakai)
</commit_message>
<xml_diff>
--- a/public/files/template/inventory/permohonan_pengadaan_barang.xlsx
+++ b/public/files/template/inventory/permohonan_pengadaan_barang.xlsx
@@ -1,63 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>PUSKESKESMAS [a.nama_puskesmas]</t>
-  </si>
-  <si>
-    <t>DAFTAR PENGADAAN / PENERIMAAN BARANG HABIS PAKAI PUSKESMAS TAHUN [a.tahun]</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>NAMA / JENIS BARANG</t>
-  </si>
-  <si>
-    <t>URAIAN BARANG</t>
-  </si>
-  <si>
-    <t>MERK/TIPE</t>
-  </si>
-  <si>
-    <t>NEGARA ASAL</t>
-  </si>
-  <si>
-    <t>VOLUME</t>
-  </si>
-  <si>
-    <t>SATUAN</t>
-  </si>
-  <si>
-    <t>HARGA SATUAN</t>
-  </si>
-  <si>
-    <t>KONDISI BARANG</t>
-  </si>
-  <si>
-    <t>BAIK</t>
-  </si>
-  <si>
-    <t>RUSAK</t>
-  </si>
-  <si>
-    <t>TIDAK DIPAKAI</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Nama / Jenis Barang</t>
+  </si>
+  <si>
+    <t>Uraian Barang</t>
+  </si>
+  <si>
+    <t>Merk / Tipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negara Asal </t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Satuan</t>
+  </si>
+  <si>
+    <t>Kondisi Barang</t>
+  </si>
+  <si>
+    <t>Baik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rusak </t>
+  </si>
+  <si>
+    <t>Tidak        di Pakai</t>
   </si>
   <si>
     <t>[a.no;block=tbs:row]</t>
@@ -69,32 +60,41 @@
     <t>[a.uraian]</t>
   </si>
   <si>
-    <t>[a.tipe]</t>
+    <t>[a.merek_tipe]</t>
   </si>
   <si>
     <t>[a.negara_asal]</t>
   </si>
   <si>
+    <t>PUSKESMAS [b.nama_puskesmas]</t>
+  </si>
+  <si>
+    <t>DAFTAR PENGADAAN / PENERIMAAN BARANG HABIS PAKAI PUSKESMAS TAHUN [b.tahun]</t>
+  </si>
+  <si>
+    <t>[a.jmlbaik]</t>
+  </si>
+  <si>
+    <t>[a.value]</t>
+  </si>
+  <si>
     <t>[a.harga]</t>
   </si>
   <si>
-    <t>[a.baik]</t>
-  </si>
-  <si>
-    <t>[a.rusak]</t>
-  </si>
-  <si>
-    <t>[a.tidakdipakai]</t>
-  </si>
-  <si>
-    <t>[a.satuan]</t>
+    <t>Harga Satuan (Rp.)</t>
+  </si>
+  <si>
+    <t>[a.jml_rusak]</t>
+  </si>
+  <si>
+    <t>[a.jml_tdkdipakai]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,22 +119,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor theme="8" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -159,14 +161,38 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="8" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="8" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="8" tint="0.39997558519241921"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -176,35 +202,42 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -283,6 +316,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -317,6 +351,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -492,198 +527,200 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="21">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="21">
-      <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="5" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C7" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D7" s="7">
         <v>4</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E7" s="7">
         <v>5</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F7" s="7">
         <v>6</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G7" s="7">
         <v>7</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="H7" s="7">
+        <v>8</v>
+      </c>
+      <c r="I7" s="7">
+        <v>9</v>
+      </c>
+      <c r="J7" s="7">
         <v>10</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="30">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="3" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="3">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3">
-        <v>7</v>
-      </c>
-      <c r="H7" s="3">
-        <v>8</v>
-      </c>
-      <c r="I7" s="3">
-        <v>9</v>
-      </c>
-      <c r="J7" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="9" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>